<commit_message>
modify tags of json and yaml
</commit_message>
<xml_diff>
--- a/appinv/out/09102989061-1.xlsx
+++ b/appinv/out/09102989061-1.xlsx
@@ -643,17 +643,16 @@
       <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s"/>
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="7">
+      <c r="E4" s="7">
         <v>110</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -662,17 +661,16 @@
       <c r="B5" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s"/>
+      <c r="C5" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="7">
+      <c r="E5" s="7">
         <v>-2.7e+01</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -763,17 +761,16 @@
       <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s"/>
+      <c r="C9" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="7">
+      <c r="E9" s="7">
         <v>65</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -864,17 +861,16 @@
       <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="6" t="s"/>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="7">
+      <c r="E13" s="7">
         <v>20</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -965,17 +961,16 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="6" t="s"/>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="7">
+      <c r="E17" s="7">
         <v>130</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1066,17 +1061,16 @@
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="6" t="s"/>
+      <c r="C21" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="7">
+      <c r="E21" s="7">
         <v>28</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1167,17 +1161,16 @@
       <c r="B25" s="6">
         <v>1</v>
       </c>
-      <c r="C25" s="6" t="s"/>
+      <c r="C25" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="7">
+      <c r="E25" s="7">
         <v>55</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>